<commit_message>
adding xlsx file and notebook for analysis
</commit_message>
<xml_diff>
--- a/Snowpits.xlsx
+++ b/Snowpits.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27424"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27425"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://ethz-my.sharepoint.com/personal/cherold_ethz_ch/Documents/AGF-212 Snow/AGF212 Report shared folder/Pits/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="516" documentId="11_AD4DB114E441178AC67DF4912694E5DE683EDF1F" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{563E5A1F-2CBC-4537-8A68-48042ED67DA1}"/>
+  <xr:revisionPtr revIDLastSave="596" documentId="11_AD4DB114E441178AC67DF4912694E5DE683EDF1F" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F99902C3-B86B-4BBC-8949-5E3860751BD0}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="205" uniqueCount="99">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="239" uniqueCount="104">
   <si>
     <t>ID</t>
   </si>
@@ -129,6 +129,9 @@
     <t>all</t>
   </si>
   <si>
+    <t>e</t>
+  </si>
+  <si>
     <t>np</t>
   </si>
   <si>
@@ -147,6 +150,9 @@
     <t>w</t>
   </si>
   <si>
+    <t>ne</t>
+  </si>
+  <si>
     <t>end</t>
   </si>
   <si>
@@ -159,9 +165,6 @@
     <t>nw</t>
   </si>
   <si>
-    <t>ne</t>
-  </si>
-  <si>
     <t>nf</t>
   </si>
   <si>
@@ -177,9 +180,6 @@
     <t>B1</t>
   </si>
   <si>
-    <t>e</t>
-  </si>
-  <si>
     <t>on windslab</t>
   </si>
   <si>
@@ -204,7 +204,7 @@
     <t>A4 on inreach alessio</t>
   </si>
   <si>
-    <t>T2</t>
+    <t>T2.1</t>
   </si>
   <si>
     <t>A3 on inreach alessio</t>
@@ -219,18 +219,18 @@
     <t>A2 on inreach alessio</t>
   </si>
   <si>
-    <t>S</t>
-  </si>
-  <si>
-    <t>S_2nd</t>
+    <t>S1.1</t>
+  </si>
+  <si>
+    <t>layers merging - photo martin</t>
+  </si>
+  <si>
+    <t>S1.2</t>
   </si>
   <si>
     <t>S2</t>
   </si>
   <si>
-    <t>ask SMB</t>
-  </si>
-  <si>
     <t>Lilleblock to find weak layer, weak layer too deep for ECT?</t>
   </si>
   <si>
@@ -240,7 +240,22 @@
     <t>B5</t>
   </si>
   <si>
-    <t>different weak layers! 57 found in LB</t>
+    <t>weak layer 57 found in LB</t>
+  </si>
+  <si>
+    <t>T2.2</t>
+  </si>
+  <si>
+    <t>weak layer at 35and 44 merged - only one PST for both</t>
+  </si>
+  <si>
+    <t>5-10 m below stake</t>
+  </si>
+  <si>
+    <t>T2.3</t>
+  </si>
+  <si>
+    <t>T2.4</t>
   </si>
   <si>
     <t>Variable</t>
@@ -369,7 +384,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFF0000"/>
+        <fgColor theme="0"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -673,15 +688,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Z66"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="K1" workbookViewId="0">
-      <selection activeCell="V15" sqref="V15"/>
+    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
+      <selection activeCell="V14" sqref="V14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.45"/>
   <cols>
     <col min="2" max="2" width="9.85546875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="11.42578125" customWidth="1"/>
+    <col min="8" max="8" width="12.5703125" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="14" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="12.42578125" customWidth="1"/>
     <col min="25" max="25" width="18.7109375" customWidth="1"/>
   </cols>
@@ -808,6 +824,12 @@
         <f>K2+L2/60</f>
         <v>15.51886</v>
       </c>
+      <c r="N2">
+        <v>288</v>
+      </c>
+      <c r="O2" t="s">
+        <v>30</v>
+      </c>
       <c r="P2">
         <v>25</v>
       </c>
@@ -815,7 +837,7 @@
         <v>25</v>
       </c>
       <c r="R2" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="S2">
         <v>40</v>
@@ -830,18 +852,18 @@
         <v>35</v>
       </c>
       <c r="W2" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="X2" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="Z2" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
     </row>
     <row r="3" spans="1:26">
       <c r="A3" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="B3">
         <v>20240227</v>
@@ -853,7 +875,7 @@
         <v>95</v>
       </c>
       <c r="E3" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="F3" t="s">
         <v>28</v>
@@ -881,6 +903,12 @@
         <f t="shared" ref="K3:M66" si="1">K3+L3/60</f>
         <v>16.194478</v>
       </c>
+      <c r="N3">
+        <v>461</v>
+      </c>
+      <c r="O3" t="s">
+        <v>37</v>
+      </c>
       <c r="P3">
         <v>5</v>
       </c>
@@ -903,18 +931,18 @@
         <v>27</v>
       </c>
       <c r="W3" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="X3" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="Z3" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
     </row>
     <row r="4" spans="1:26">
       <c r="A4" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="B4">
         <v>20240229</v>
@@ -926,7 +954,7 @@
         <v>102</v>
       </c>
       <c r="E4" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="F4" t="s">
         <v>28</v>
@@ -958,42 +986,45 @@
         <v>503</v>
       </c>
       <c r="O4" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="P4">
         <v>6</v>
       </c>
       <c r="Q4" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="R4" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="S4" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="T4" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="U4" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="V4" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="W4" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="X4" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="Y4" t="s">
-        <v>44</v>
+        <v>45</v>
+      </c>
+      <c r="Z4" t="s">
+        <v>45</v>
       </c>
     </row>
     <row r="5" spans="1:26">
       <c r="A5" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="B5">
         <v>20240228</v>
@@ -1005,10 +1036,10 @@
         <v>122</v>
       </c>
       <c r="E5" t="s">
-        <v>46</v>
+        <v>30</v>
       </c>
       <c r="F5" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="G5" t="s">
         <v>29</v>
@@ -1017,11 +1048,11 @@
         <v>78.210171666666668</v>
       </c>
       <c r="I5" s="2">
-        <v>12.616400000000001</v>
+        <v>0</v>
       </c>
       <c r="J5">
         <f t="shared" si="0"/>
-        <v>78.420445000000001</v>
+        <v>78.210171666666668</v>
       </c>
       <c r="K5">
         <v>15.62862</v>
@@ -1037,7 +1068,7 @@
         <v>107</v>
       </c>
       <c r="O5" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="P5">
         <v>18</v>
@@ -1061,10 +1092,10 @@
         <v>44</v>
       </c>
       <c r="W5" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="X5" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="Z5" t="s">
         <v>47</v>
@@ -1084,7 +1115,7 @@
         <v>103</v>
       </c>
       <c r="E6" t="s">
-        <v>46</v>
+        <v>30</v>
       </c>
       <c r="F6" t="s">
         <v>28</v>
@@ -1116,19 +1147,19 @@
         <v>107</v>
       </c>
       <c r="O6" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="P6">
         <v>22</v>
       </c>
       <c r="Q6" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="R6" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="S6" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="T6">
         <v>95</v>
@@ -1140,10 +1171,10 @@
         <v>26</v>
       </c>
       <c r="W6" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="X6" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="Z6" t="s">
         <v>49</v>
@@ -1163,7 +1194,7 @@
         <v>165</v>
       </c>
       <c r="E7" t="s">
-        <v>46</v>
+        <v>30</v>
       </c>
       <c r="F7" t="s">
         <v>28</v>
@@ -1195,7 +1226,7 @@
         <v>107</v>
       </c>
       <c r="O7" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="P7">
         <v>18</v>
@@ -1219,10 +1250,10 @@
         <v>40</v>
       </c>
       <c r="W7" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="X7" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="Z7" t="s">
         <v>51</v>
@@ -1242,7 +1273,7 @@
         <v>99</v>
       </c>
       <c r="E8" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="F8" t="s">
         <v>28</v>
@@ -1273,6 +1304,9 @@
       <c r="N8">
         <v>448</v>
       </c>
+      <c r="O8" t="s">
+        <v>37</v>
+      </c>
       <c r="P8">
         <v>7</v>
       </c>
@@ -1295,10 +1329,10 @@
         <v>38</v>
       </c>
       <c r="W8" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="X8" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="Y8" t="s">
         <v>54</v>
@@ -1318,7 +1352,7 @@
         <v>115</v>
       </c>
       <c r="E9" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="F9" t="s">
         <v>28</v>
@@ -1349,6 +1383,9 @@
       <c r="N9">
         <v>350</v>
       </c>
+      <c r="O9" t="s">
+        <v>30</v>
+      </c>
       <c r="P9">
         <v>5</v>
       </c>
@@ -1371,10 +1408,10 @@
         <v>50</v>
       </c>
       <c r="W9" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="X9" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="Y9" t="s">
         <v>56</v>
@@ -1394,7 +1431,7 @@
         <v>54</v>
       </c>
       <c r="E10" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="F10" t="s">
         <v>28</v>
@@ -1450,10 +1487,10 @@
         <v>50</v>
       </c>
       <c r="W10" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="X10" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="Y10" t="s">
         <v>59</v>
@@ -1473,10 +1510,10 @@
         <v>160</v>
       </c>
       <c r="E11" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="F11" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="G11" t="s">
         <v>29</v>
@@ -1501,8 +1538,11 @@
         <f t="shared" si="1"/>
         <v>16.142171666666666</v>
       </c>
+      <c r="N11">
+        <v>648</v>
+      </c>
       <c r="O11" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="P11">
         <v>22</v>
@@ -1511,7 +1551,7 @@
         <v>14</v>
       </c>
       <c r="R11" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="S11">
         <v>29</v>
@@ -1526,15 +1566,18 @@
         <v>29</v>
       </c>
       <c r="W11" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="X11" t="s">
-        <v>43</v>
+        <v>44</v>
+      </c>
+      <c r="Y11" t="s">
+        <v>61</v>
       </c>
     </row>
     <row r="12" spans="1:26">
       <c r="A12" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="B12">
         <v>20230302</v>
@@ -1546,10 +1589,10 @@
         <v>160</v>
       </c>
       <c r="E12" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="F12" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="G12" t="s">
         <v>29</v>
@@ -1574,8 +1617,11 @@
         <f t="shared" si="1"/>
         <v>16.142171666666666</v>
       </c>
+      <c r="N12">
+        <v>648</v>
+      </c>
       <c r="O12" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="P12">
         <v>22</v>
@@ -1584,7 +1630,7 @@
         <v>24</v>
       </c>
       <c r="R12" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="S12">
         <v>35</v>
@@ -1599,15 +1645,15 @@
         <v>35</v>
       </c>
       <c r="W12" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="X12" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
     </row>
     <row r="13" spans="1:26">
       <c r="A13" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="B13">
         <v>20240302</v>
@@ -1619,10 +1665,10 @@
         <v>120</v>
       </c>
       <c r="E13" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="F13" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="G13" t="s">
         <v>29</v>
@@ -1644,11 +1690,14 @@
         <v>6.9386000000000001</v>
       </c>
       <c r="M13">
-        <f t="shared" si="1"/>
+        <f>K13+L13/60</f>
         <v>16.115643333333335</v>
       </c>
+      <c r="N13">
+        <v>735</v>
+      </c>
       <c r="O13" t="s">
-        <v>46</v>
+        <v>30</v>
       </c>
       <c r="P13">
         <v>24</v>
@@ -1672,10 +1721,10 @@
         <v>43</v>
       </c>
       <c r="W13" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="X13" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
     </row>
     <row r="14" spans="1:26">
@@ -1688,14 +1737,14 @@
       <c r="C14">
         <v>1500</v>
       </c>
-      <c r="D14" t="s">
-        <v>63</v>
+      <c r="D14">
+        <v>112</v>
       </c>
       <c r="E14" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="F14" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="G14" t="s">
         <v>29</v>
@@ -1717,20 +1766,26 @@
         <v>3.8159000000000001</v>
       </c>
       <c r="M14">
-        <f t="shared" si="1"/>
+        <f>K14+L14/60</f>
         <v>16.063598333333335</v>
+      </c>
+      <c r="N14">
+        <v>547</v>
+      </c>
+      <c r="O14" t="s">
+        <v>36</v>
       </c>
       <c r="P14">
         <v>6</v>
       </c>
       <c r="Q14" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="R14" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="S14" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="T14">
         <v>53</v>
@@ -1742,10 +1797,10 @@
         <v>53</v>
       </c>
       <c r="W14" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="X14" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="Y14" t="s">
         <v>64</v>
@@ -1764,14 +1819,14 @@
       <c r="C15">
         <v>1545</v>
       </c>
-      <c r="D15" t="s">
-        <v>63</v>
+      <c r="D15">
+        <v>126</v>
       </c>
       <c r="E15" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="F15" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="G15" t="s">
         <v>29</v>
@@ -1796,6 +1851,12 @@
         <f t="shared" si="1"/>
         <v>16.083805000000002</v>
       </c>
+      <c r="N15">
+        <v>601</v>
+      </c>
+      <c r="O15" t="s">
+        <v>36</v>
+      </c>
       <c r="P15">
         <v>5</v>
       </c>
@@ -1803,7 +1864,7 @@
         <v>9</v>
       </c>
       <c r="R15" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="S15">
         <v>10</v>
@@ -1815,13 +1876,13 @@
         <v>100</v>
       </c>
       <c r="V15" s="3">
-        <v>57</v>
+        <v>10</v>
       </c>
       <c r="W15" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="X15" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="Y15" t="s">
         <v>67</v>
@@ -1831,36 +1892,249 @@
       </c>
     </row>
     <row r="16" spans="1:26">
+      <c r="A16" t="s">
+        <v>68</v>
+      </c>
+      <c r="B16">
+        <v>20240303</v>
+      </c>
+      <c r="C16">
+        <v>1145</v>
+      </c>
+      <c r="D16">
+        <v>117</v>
+      </c>
+      <c r="E16" t="s">
+        <v>36</v>
+      </c>
+      <c r="F16" t="s">
+        <v>43</v>
+      </c>
+      <c r="G16" t="s">
+        <v>29</v>
+      </c>
+      <c r="H16">
+        <v>78</v>
+      </c>
+      <c r="I16">
+        <v>15.407999999999999</v>
+      </c>
       <c r="J16">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>78.256799999999998</v>
+      </c>
+      <c r="K16">
+        <v>16</v>
+      </c>
+      <c r="L16">
+        <v>13.8401</v>
       </c>
       <c r="M16">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="17" spans="10:13">
+        <v>16.230668333333334</v>
+      </c>
+      <c r="N16">
+        <v>446</v>
+      </c>
+      <c r="O16" t="s">
+        <v>37</v>
+      </c>
+      <c r="P16">
+        <v>5</v>
+      </c>
+      <c r="Q16">
+        <v>21</v>
+      </c>
+      <c r="R16">
+        <v>21</v>
+      </c>
+      <c r="S16">
+        <v>35</v>
+      </c>
+      <c r="T16">
+        <v>98</v>
+      </c>
+      <c r="U16">
+        <v>100</v>
+      </c>
+      <c r="V16">
+        <v>35</v>
+      </c>
+      <c r="W16" t="s">
+        <v>38</v>
+      </c>
+      <c r="X16" t="s">
+        <v>33</v>
+      </c>
+      <c r="Y16" t="s">
+        <v>69</v>
+      </c>
+      <c r="Z16" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="17" spans="1:26">
+      <c r="A17" t="s">
+        <v>71</v>
+      </c>
+      <c r="B17">
+        <v>20240303</v>
+      </c>
+      <c r="C17">
+        <v>1145</v>
+      </c>
+      <c r="D17">
+        <v>117</v>
+      </c>
+      <c r="E17" t="s">
+        <v>36</v>
+      </c>
+      <c r="F17" t="s">
+        <v>43</v>
+      </c>
+      <c r="G17" t="s">
+        <v>29</v>
+      </c>
+      <c r="H17">
+        <v>78</v>
+      </c>
+      <c r="I17">
+        <v>15.407999999999999</v>
+      </c>
       <c r="J17">
-        <f t="shared" si="0"/>
-        <v>0</v>
+        <f>H17+I17/60</f>
+        <v>78.256799999999998</v>
+      </c>
+      <c r="K17">
+        <v>16</v>
+      </c>
+      <c r="L17">
+        <v>13.8401</v>
       </c>
       <c r="M17">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="18" spans="10:13">
+        <f>K17+L17/60</f>
+        <v>16.230668333333334</v>
+      </c>
+      <c r="N17">
+        <v>446</v>
+      </c>
+      <c r="O17" t="s">
+        <v>37</v>
+      </c>
+      <c r="P17">
+        <v>5</v>
+      </c>
+      <c r="Q17">
+        <v>24</v>
+      </c>
+      <c r="R17" t="s">
+        <v>31</v>
+      </c>
+      <c r="S17">
+        <v>44</v>
+      </c>
+      <c r="T17">
+        <v>98</v>
+      </c>
+      <c r="U17">
+        <v>100</v>
+      </c>
+      <c r="V17">
+        <v>35</v>
+      </c>
+      <c r="W17" t="s">
+        <v>38</v>
+      </c>
+      <c r="X17" t="s">
+        <v>33</v>
+      </c>
+      <c r="Y17" t="s">
+        <v>69</v>
+      </c>
+      <c r="Z17" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="18" spans="1:26">
+      <c r="A18" t="s">
+        <v>72</v>
+      </c>
+      <c r="B18">
+        <v>20240303</v>
+      </c>
+      <c r="C18">
+        <v>1145</v>
+      </c>
+      <c r="D18">
+        <v>117</v>
+      </c>
+      <c r="E18" t="s">
+        <v>36</v>
+      </c>
+      <c r="F18" t="s">
+        <v>43</v>
+      </c>
+      <c r="G18" t="s">
+        <v>29</v>
+      </c>
+      <c r="H18">
+        <v>78</v>
+      </c>
+      <c r="I18">
+        <v>15.407999999999999</v>
+      </c>
       <c r="J18">
-        <f t="shared" si="0"/>
-        <v>0</v>
+        <f>H18+I18/60</f>
+        <v>78.256799999999998</v>
+      </c>
+      <c r="K18">
+        <v>16</v>
+      </c>
+      <c r="L18">
+        <v>13.8401</v>
       </c>
       <c r="M18">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="19" spans="10:13">
+        <f>K18+L18/60</f>
+        <v>16.230668333333334</v>
+      </c>
+      <c r="N18">
+        <v>446</v>
+      </c>
+      <c r="O18" t="s">
+        <v>37</v>
+      </c>
+      <c r="P18">
+        <v>5</v>
+      </c>
+      <c r="Q18">
+        <v>25</v>
+      </c>
+      <c r="R18" t="s">
+        <v>31</v>
+      </c>
+      <c r="S18">
+        <v>53</v>
+      </c>
+      <c r="T18">
+        <v>59</v>
+      </c>
+      <c r="U18">
+        <v>100</v>
+      </c>
+      <c r="V18">
+        <v>53</v>
+      </c>
+      <c r="W18" t="s">
+        <v>38</v>
+      </c>
+      <c r="X18" t="s">
+        <v>33</v>
+      </c>
+      <c r="Z18" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="19" spans="1:26">
       <c r="J19">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -1870,7 +2144,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="10:13">
+    <row r="20" spans="1:26">
       <c r="J20">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -1880,7 +2154,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="10:13">
+    <row r="21" spans="1:26">
       <c r="J21">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -1890,7 +2164,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="10:13">
+    <row r="22" spans="1:26">
       <c r="J22">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -1900,7 +2174,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="10:13">
+    <row r="23" spans="1:26">
       <c r="J23">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -1910,7 +2184,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="10:13">
+    <row r="24" spans="1:26">
       <c r="J24">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -1920,7 +2194,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="10:13">
+    <row r="25" spans="1:26">
       <c r="J25">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -1930,7 +2204,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="10:13">
+    <row r="26" spans="1:26">
       <c r="J26">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -1940,7 +2214,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="10:13">
+    <row r="27" spans="1:26">
       <c r="J27">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -1950,7 +2224,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="10:13">
+    <row r="28" spans="1:26">
       <c r="J28">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -1960,7 +2234,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="10:13">
+    <row r="29" spans="1:26">
       <c r="J29">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -1970,7 +2244,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="10:13">
+    <row r="30" spans="1:26">
       <c r="J30">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -1980,7 +2254,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="10:13">
+    <row r="31" spans="1:26">
       <c r="J31">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -1990,7 +2264,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="10:13">
+    <row r="32" spans="1:26">
       <c r="J32">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -2362,13 +2636,13 @@
   <sheetData>
     <row r="1" spans="1:3" s="1" customFormat="1">
       <c r="A1" s="1" t="s">
-        <v>68</v>
+        <v>73</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>69</v>
+        <v>74</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>70</v>
+        <v>75</v>
       </c>
     </row>
     <row r="2" spans="1:3">
@@ -2384,7 +2658,7 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>71</v>
+        <v>76</v>
       </c>
     </row>
     <row r="4" spans="1:3">
@@ -2392,7 +2666,7 @@
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>72</v>
+        <v>77</v>
       </c>
     </row>
     <row r="5" spans="1:3">
@@ -2400,7 +2674,7 @@
         <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>73</v>
+        <v>78</v>
       </c>
     </row>
     <row r="6" spans="1:3">
@@ -2408,10 +2682,10 @@
         <v>4</v>
       </c>
       <c r="B6" t="s">
-        <v>74</v>
+        <v>79</v>
       </c>
       <c r="C6" t="s">
-        <v>75</v>
+        <v>80</v>
       </c>
     </row>
     <row r="7" spans="1:3">
@@ -2419,10 +2693,10 @@
         <v>5</v>
       </c>
       <c r="B7" t="s">
-        <v>76</v>
+        <v>81</v>
       </c>
       <c r="C7" t="s">
-        <v>77</v>
+        <v>82</v>
       </c>
     </row>
     <row r="8" spans="1:3">
@@ -2430,10 +2704,10 @@
         <v>6</v>
       </c>
       <c r="B8" t="s">
-        <v>78</v>
+        <v>83</v>
       </c>
       <c r="C8" t="s">
-        <v>79</v>
+        <v>84</v>
       </c>
     </row>
     <row r="9" spans="1:3">
@@ -2441,7 +2715,7 @@
         <v>7</v>
       </c>
       <c r="B9" t="s">
-        <v>80</v>
+        <v>85</v>
       </c>
     </row>
     <row r="10" spans="1:3">
@@ -2449,7 +2723,7 @@
         <v>8</v>
       </c>
       <c r="B10" t="s">
-        <v>81</v>
+        <v>86</v>
       </c>
     </row>
     <row r="11" spans="1:3">
@@ -2457,7 +2731,7 @@
         <v>9</v>
       </c>
       <c r="B11" t="s">
-        <v>82</v>
+        <v>87</v>
       </c>
     </row>
     <row r="12" spans="1:3">
@@ -2465,7 +2739,7 @@
         <v>10</v>
       </c>
       <c r="B12" t="s">
-        <v>83</v>
+        <v>88</v>
       </c>
     </row>
     <row r="13" spans="1:3">
@@ -2473,7 +2747,7 @@
         <v>11</v>
       </c>
       <c r="B13" t="s">
-        <v>84</v>
+        <v>89</v>
       </c>
     </row>
     <row r="14" spans="1:3">
@@ -2481,7 +2755,7 @@
         <v>12</v>
       </c>
       <c r="B14" t="s">
-        <v>85</v>
+        <v>90</v>
       </c>
     </row>
     <row r="15" spans="1:3">
@@ -2489,7 +2763,7 @@
         <v>15</v>
       </c>
       <c r="B15" t="s">
-        <v>86</v>
+        <v>91</v>
       </c>
     </row>
     <row r="16" spans="1:3">
@@ -2497,7 +2771,7 @@
         <v>16</v>
       </c>
       <c r="B16" t="s">
-        <v>87</v>
+        <v>92</v>
       </c>
     </row>
     <row r="17" spans="1:3">
@@ -2505,7 +2779,7 @@
         <v>17</v>
       </c>
       <c r="B17" t="s">
-        <v>88</v>
+        <v>93</v>
       </c>
     </row>
     <row r="18" spans="1:3">
@@ -2513,7 +2787,7 @@
         <v>18</v>
       </c>
       <c r="B18" t="s">
-        <v>89</v>
+        <v>94</v>
       </c>
     </row>
     <row r="19" spans="1:3">
@@ -2521,7 +2795,7 @@
         <v>19</v>
       </c>
       <c r="B19" t="s">
-        <v>90</v>
+        <v>95</v>
       </c>
     </row>
     <row r="20" spans="1:3">
@@ -2529,7 +2803,7 @@
         <v>20</v>
       </c>
       <c r="B20" t="s">
-        <v>91</v>
+        <v>96</v>
       </c>
     </row>
     <row r="21" spans="1:3">
@@ -2537,7 +2811,7 @@
         <v>21</v>
       </c>
       <c r="B21" t="s">
-        <v>92</v>
+        <v>97</v>
       </c>
     </row>
     <row r="22" spans="1:3">
@@ -2545,10 +2819,10 @@
         <v>22</v>
       </c>
       <c r="B22" t="s">
-        <v>93</v>
+        <v>98</v>
       </c>
       <c r="C22" t="s">
-        <v>94</v>
+        <v>99</v>
       </c>
     </row>
     <row r="23" spans="1:3">
@@ -2556,10 +2830,10 @@
         <v>23</v>
       </c>
       <c r="B23" t="s">
-        <v>95</v>
+        <v>100</v>
       </c>
       <c r="C23" t="s">
-        <v>96</v>
+        <v>101</v>
       </c>
     </row>
     <row r="24" spans="1:3">
@@ -2567,7 +2841,7 @@
         <v>24</v>
       </c>
       <c r="B24" t="s">
-        <v>97</v>
+        <v>102</v>
       </c>
     </row>
     <row r="25" spans="1:3">
@@ -2575,7 +2849,7 @@
         <v>25</v>
       </c>
       <c r="B25" t="s">
-        <v>98</v>
+        <v>103</v>
       </c>
     </row>
   </sheetData>

</xml_diff>